<commit_message>
Deploying to gh-pages from @ tklammsteiner/tklammsteiner.github.io@9f3c80c4b1be95ed8e76125f1209316066365a15 🚀
</commit_message>
<xml_diff>
--- a/assets/data/bugbook.xlsx
+++ b/assets/data/bugbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Github\tklammsteiner.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D2DCB4-876A-40D3-9B35-6524E85CCE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CBD3A8-B41E-484B-B6DE-AF23FC655178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chapters" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="230">
   <si>
     <t xml:space="preserve"> Basic information and good practices on how to maintain a stock population for &lt;i&gt;Tenebrio molitor&lt;/i&gt; and &lt;i&gt;Hermetia illucens&lt;/i&gt; for research</t>
   </si>
@@ -121,9 +121,6 @@
     <t>DOI</t>
   </si>
   <si>
-    <t>In recent decades, research on insect production for food and feed has expanded significantly, driven by advances in farming, processing, genetics, and sustainability. A wide range of data analysis methods, from traditional statistical techniques to advanced machine learning algorithms, have been employed to optimize various aspects of insect-based systems. In production, methods like analysis of variance (ANOVA) and regression analysis help improve breeding conditions and growth rates, while multivariate analyses support processing studies by evaluating nutritional and microbial safety. Genetic research leverages bioinformatics, genome-wide association studies (GWAS), and quantitative genetics to enhance traits like yield and disease resistance. Sustainability assessments use life cycle analysis (LCA) with Monte Carlo simulations to measure environmental impacts. Emerging tools, such as neural networks and support vector machines, are gaining traction for predicting feed conversion ratios and disease detection. Despite this progress, the field lacks a comprehensive guide to systematically bridge classic and novel data analysis methods specific to insect research. This study aims to address this gap by offering an accessible manual for researchers and professionals. It will consolidate methodologies across disciplines, highlighting foundational tools for beginners while showcasing advanced techniques for experts. Topics include the application of tailored methods like chitin and protein accounting, sensory analysis, consumer preference modelling, and data visualization to improve stakeholder communication. By enhancing methodological rigor and fostering transparency, this guide will promote innovation, facilitate data interchange, and ensure the replicability of findings. Ultimately, it aims to drive sustainable advancements in the mass production of insects for food and feed.</t>
-  </si>
-  <si>
     <t>First_Author</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>J.K. Tomberlin, T. Klammsteiner, N. Lemke, P. Yadav, C. Sandrock</t>
   </si>
   <si>
-    <t>Behavioural research and its applications has a rich history in science with direct applications continuing to expand global understanding of ecosystem function, structure, and evolution. The same can be said for such research as related to the applied sciences including entomology. The purpose of this chapter is to provide context to various approaches for assessing behaviour of insects that are mass produced for food and feed. By using the black soldier fly as a model, various approaches for conducting such research are explored along with providing some perspective as the value of such data for optimising insect production.</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -692,6 +686,39 @@
   </si>
   <si>
     <t>Universidad de Vigo</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1163/23524588-bja10209</t>
+  </si>
+  <si>
+    <t>D.G.A.B. Oonincx, M. Gold, G. Bosch, J.B. Guillaume, C.I. Rumbos, S. Naser El Deen, C. Sandrock, S. Bellezza Oddon, C.G. Athanassiou, M. Cambra-López, J.J. Pascual, A.P. Parodi, T. Spranghers, W. Yakti</t>
+  </si>
+  <si>
+    <t>The rapid expansion of insect farming as a sustainable approach for protein production has led to an accumulation of published research on the use of low-value substrates as insect feed. However, compared to conventional livestock, there is a lack of fundamental knowledge about the nutritional physiology and requirements of insects. Such knowledge can lead to the development of optimised feeding substrates that boost insect performance and nutrient composition. In this chapter, the current knowledge on the nutritional requirements of the most relevant insects produced for food and feed is reviewed, and the methods and assays used to investigate the specific requirements are presented. This description of current knowledge on nutritional requirements of edible insects can be used to design suitable rearing diets and as a foundation to further our understanding of insect nutrition.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1163/23524588-bja10226</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Coleoptera, Diptera, edible insects, nutrient requirements, Orthoptera</t>
+  </si>
+  <si>
+    <t>data analysis methods, genetic research, insect production, machine learning, sustainability assessment</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1163/23524588-bja10225</t>
+  </si>
+  <si>
+    <t>Behavioural research and its applications has a rich history in science with direct applications continuing to expand global understanding of ecosystem function, structure, and evolution. The same can be said for such research as related to the applied sciences including entomology. The purpose of this chapter is to provide context to various approaches for assessing behaviour of insects that are mass produced for food and feed. By using the black soldier fly as a model, various approaches for conducting such research are explored along with providing some perspective on the value of such data for optimising insect production. However, it should be noted that this chapter is not exhaustive with regards to variables that can be examined, or the methods employed.</t>
+  </si>
+  <si>
+    <t>In recent decades, research on insect production for food and feed has expanded significantly, driven by advances in farming, processing, genetics, and sustainability. Various data analysis methods, from traditional statistics to advanced machine learning, are used to optimise aspects of insect-based systems. In production, methods like analysis of variance (ANOVA) and regression analysis help improve breeding conditions and growth rates, while multivariate analyses support processing studies by evaluating nutritional and microbial safety. Genetic research leverages bioinformatics, genome-wide association studies (GWAS), and quantitative genetics to enhance traits like yield and disease resistance. Sustainability assessments use life cycle analysis (LCA) with Monte Carlo simulations to measure environmental impacts. Emerging tools, such as neural networks and support vector machines, are gaining traction for predicting feed conversion ratios and disease detection. Despite progress, a comprehensive guide that bridges classic and novel data analysis methods in insect research is still lacking. This study aims to address this gap by offering an accessible manual for researchers and professionals. It will consolidate methodologies across disciplines, highlighting foundational tools for beginners while showcasing advanced techniques for experts. Topics include the application of tailored methods like chitin and protein accounting, sensory analysis, consumer preference modelling, and data visualisation to improve stakeholder communication. By enhancing methodological rigor and fostering transparency, this guide will promote innovation, facilitate data interchange, and ensure the replicability of findings. Ultimately, it aims to drive sustainable advancements in the mass production of insects for food and feed.</t>
+  </si>
+  <si>
+    <t>choice test, electrophysiology, ethology, experimental design, reproduction</t>
   </si>
 </sst>
 </file>
@@ -765,7 +792,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1043,29 +1070,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.26953125" style="1" customWidth="1"/>
     <col min="3" max="3" width="127" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.6328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.6328125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -1074,13 +1101,16 @@
         <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1091,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1102,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1113,7 +1143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1123,14 +1153,20 @@
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1141,7 +1177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1152,13 +1188,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1169,10 +1205,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1183,7 +1219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1193,8 +1229,20 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1205,7 +1253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1216,7 +1264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1227,7 +1275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1237,11 +1285,17 @@
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>30</v>
+        <v>228</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -1253,11 +1307,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9512CDD1-224C-42FF-A8C0-1743894FC8B7}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.81640625" customWidth="1"/>
     <col min="2" max="3" width="13.90625" customWidth="1"/>
@@ -1267,16 +1321,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>12</v>
@@ -1284,216 +1338,216 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
@@ -1501,10 +1555,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E16" s="5">
         <v>3</v>
@@ -1512,10 +1566,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E17" s="5">
         <v>3</v>
@@ -1523,10 +1577,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -1534,10 +1588,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E19" s="5">
         <v>3</v>
@@ -1545,44 +1599,44 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E22" s="5">
         <v>4</v>
@@ -1590,47 +1644,47 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E25" s="5">
         <v>4</v>
@@ -1638,10 +1692,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E26" s="5">
         <v>5</v>
@@ -1649,10 +1703,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E27" s="5">
         <v>5</v>
@@ -1660,10 +1714,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E28" s="5">
         <v>5</v>
@@ -1671,10 +1725,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E29" s="5">
         <v>5</v>
@@ -1682,10 +1736,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E30" s="5">
         <v>5</v>
@@ -1693,7 +1747,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E31" s="5">
         <v>5</v>
@@ -1701,10 +1755,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E32" s="5">
         <v>5</v>
@@ -1712,7 +1766,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E33" s="5">
         <v>5</v>
@@ -1720,7 +1774,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E34" s="5">
         <v>5</v>
@@ -1728,10 +1782,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E35" s="5">
         <v>5</v>
@@ -1739,10 +1793,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E36" s="5">
         <v>5</v>
@@ -1750,16 +1804,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E37" s="5">
         <v>5</v>
@@ -1767,7 +1821,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E38" s="5">
         <v>5</v>
@@ -1775,10 +1829,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E39" s="5">
         <v>5</v>
@@ -1786,10 +1840,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E40" s="5">
         <v>5</v>
@@ -1797,7 +1851,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E41" s="5">
         <v>5</v>
@@ -1805,10 +1859,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E42" s="5">
         <v>5</v>
@@ -1816,10 +1870,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E43" s="5">
         <v>5</v>
@@ -1827,10 +1881,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E44" s="5">
         <v>5</v>
@@ -1838,10 +1892,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E45" s="5">
         <v>5</v>
@@ -1849,10 +1903,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E46" s="5">
         <v>5</v>
@@ -1860,16 +1914,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D47" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E47" s="5">
         <v>6</v>
@@ -1877,16 +1931,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C48" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E48" s="5">
         <v>6</v>
@@ -1894,16 +1948,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D49" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E49" s="5">
         <v>6</v>
@@ -1911,16 +1965,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D50" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E50" s="5">
         <v>6</v>
@@ -1928,16 +1982,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D51" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E51" s="5">
         <v>6</v>
@@ -1945,16 +1999,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D52" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E52" s="5">
         <v>6</v>
@@ -1962,16 +2016,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D53" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E53" s="5">
         <v>6</v>
@@ -1979,10 +2033,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E54" s="5">
         <v>7</v>
@@ -1990,10 +2044,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E55" s="5">
         <v>7</v>
@@ -2001,16 +2055,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C56" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D56" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E56" s="5">
         <v>7</v>
@@ -2018,16 +2072,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D57" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E57" s="5">
         <v>8</v>
@@ -2035,10 +2089,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E58" s="5">
         <v>8</v>
@@ -2046,10 +2100,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E59" s="5">
         <v>8</v>
@@ -2057,27 +2111,27 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D60" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E61" s="5">
         <v>8</v>
@@ -2085,10 +2139,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E62" s="5">
         <v>8</v>
@@ -2096,10 +2150,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E63" s="5">
         <v>8</v>
@@ -2107,10 +2161,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E64" s="5">
         <v>8</v>
@@ -2118,21 +2172,21 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E66" s="5">
         <v>8</v>
@@ -2140,10 +2194,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E67" s="5">
         <v>8</v>
@@ -2151,10 +2205,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E68" s="5">
         <v>8</v>
@@ -2162,10 +2216,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E69" s="5">
         <v>8</v>
@@ -2173,16 +2227,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D70" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E70" s="5">
         <v>8</v>
@@ -2190,16 +2244,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C71" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D71" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E71" s="5">
         <v>13</v>
@@ -2207,10 +2261,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E72" s="5">
         <v>13</v>
@@ -2218,10 +2272,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B73" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E73" s="5">
         <v>11</v>
@@ -2229,10 +2283,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E74" s="5">
         <v>11</v>
@@ -2240,10 +2294,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E75" s="5">
         <v>11</v>
@@ -2251,16 +2305,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B76" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C76" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D76" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E76" s="5">
         <v>11</v>
@@ -2268,10 +2322,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E77" s="5">
         <v>11</v>
@@ -2279,16 +2333,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D78" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E78" s="5">
         <v>11</v>
@@ -2296,10 +2350,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E79" s="5">
         <v>11</v>
@@ -2307,16 +2361,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C80" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D80" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E80" s="5">
         <v>11</v>
@@ -2324,10 +2378,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E81" s="5">
         <v>11</v>
@@ -2335,10 +2389,10 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B82" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E82" s="5">
         <v>11</v>
@@ -2346,10 +2400,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B83" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E83" s="5">
         <v>11</v>
@@ -2357,16 +2411,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B84" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" t="s">
+        <v>192</v>
+      </c>
+      <c r="D84" t="s">
         <v>193</v>
-      </c>
-      <c r="B84" t="s">
-        <v>139</v>
-      </c>
-      <c r="C84" t="s">
-        <v>194</v>
-      </c>
-      <c r="D84" t="s">
-        <v>195</v>
       </c>
       <c r="E84" s="5">
         <v>11</v>
@@ -2374,10 +2428,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E85" s="5">
         <v>11</v>
@@ -2385,7 +2439,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E86" s="5">
         <v>11</v>
@@ -2393,10 +2447,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E87" s="5">
         <v>11</v>
@@ -2404,10 +2458,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E88" s="5">
         <v>11</v>
@@ -2415,16 +2469,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B89" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C89" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D89" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E89" s="5">
         <v>12</v>
@@ -2432,16 +2486,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B90" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C90" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D90" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E90" s="5">
         <v>12</v>
@@ -2449,16 +2503,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B91" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C91" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D91" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E91" s="5">
         <v>12</v>
@@ -2466,24 +2520,24 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B93" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C93" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D93" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E93" s="5">
         <v>9</v>
@@ -2491,16 +2545,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B94" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C94" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D94" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E94" s="5">
         <v>9</v>
@@ -2508,16 +2562,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B95" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C95" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D95" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E95" s="5">
         <v>10</v>
@@ -2525,16 +2579,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C96" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D96" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E96" s="5">
         <v>10</v>
@@ -2542,10 +2596,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E97" s="5">
         <v>10</v>
@@ -2553,10 +2607,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B98" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E98" s="5">
         <v>10</v>
@@ -2564,10 +2618,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E99" s="5">
         <v>10</v>
@@ -2575,10 +2629,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B100" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E100" s="5">
         <v>10</v>
@@ -2586,10 +2640,10 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B101" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E101" s="5">
         <v>10</v>
@@ -2597,16 +2651,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B102" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C102" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E102" s="5">
         <v>10</v>

</xml_diff>